<commit_message>
Edición de multiples páginas y ajuste primeras dos páginas
</commit_message>
<xml_diff>
--- a/files/Data.xlsx
+++ b/files/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abels\OneDrive\Desktop\Generador-Solicitudes\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F28A8-CAF8-40D8-84CD-CF0FCABC7EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3FDA93-0BC5-417E-88FE-4D42B771B292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7171335B-6EB2-4E13-BF21-E8880F3867D1}"/>
   </bookViews>
@@ -183,13 +183,13 @@
     <t>Calle López</t>
   </si>
   <si>
-    <t>17 de marzo de 2022</t>
-  </si>
-  <si>
-    <t>18 de septiembre de 2022</t>
-  </si>
-  <si>
-    <t>07 de noviembre de 2022</t>
+    <t>17 del 03 del 2022</t>
+  </si>
+  <si>
+    <t>18 del 09 del 2022</t>
+  </si>
+  <si>
+    <t>07 del 11 del 2022</t>
   </si>
 </sst>
 </file>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F700F14-4C69-4246-A617-9B75CEA3E3EC}">
   <dimension ref="A1:Y131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Últimos ajustes primera página
</commit_message>
<xml_diff>
--- a/files/Data.xlsx
+++ b/files/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abels\OneDrive\Desktop\Generador-Solicitudes\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3FDA93-0BC5-417E-88FE-4D42B771B292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB00E7FD-3981-4A5F-9179-DD0B54493BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7171335B-6EB2-4E13-BF21-E8880F3867D1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Fecha de Solicitud</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>07 del 11 del 2022</t>
+  </si>
+  <si>
+    <t>Esta es una observación de prueba innecesariamente larga</t>
+  </si>
+  <si>
+    <t>Esta es una observación de prueba</t>
+  </si>
+  <si>
+    <t>Esta es una observación de prueba innecesariamente larga con el propósito de hacer un test de acomodo de texto muy muy larga, un poco demasiado, por no decir exageradamente larga. Este es el límite del texto</t>
   </si>
 </sst>
 </file>
@@ -788,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F700F14-4C69-4246-A617-9B75CEA3E3EC}">
   <dimension ref="A1:Y131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +1002,9 @@
       <c r="X3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="7"/>
+      <c r="Y3" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
@@ -1068,6 +1079,9 @@
       <c r="X4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="Y4" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
@@ -1141,6 +1155,9 @@
       </c>
       <c r="X5" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix (generador_pdf): new design
</commit_message>
<xml_diff>
--- a/files/Data.xlsx
+++ b/files/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Molina\Documents\MEGA\+Generadores\Solicitudes_rev3\PDF-Request-Generator-master\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abels\OneDrive\Desktop\PDF-Request-Generator\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CC31BB-566A-430D-B762-04C1972DEBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276BCE9F-DE83-4695-93DC-D4868D3813D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{7171335B-6EB2-4E13-BF21-E8880F3867D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7171335B-6EB2-4E13-BF21-E8880F3867D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,9 +543,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -583,7 +583,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -689,7 +689,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -831,7 +831,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -841,29 +841,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F700F14-4C69-4246-A617-9B75CEA3E3EC}">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.54296875" style="2" customWidth="1"/>
-    <col min="5" max="8" width="10.81640625" style="3"/>
-    <col min="9" max="9" width="11.453125" style="3"/>
-    <col min="10" max="10" width="33.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.7265625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" style="4" customWidth="1"/>
-    <col min="13" max="14" width="30.54296875" style="4" customWidth="1"/>
-    <col min="15" max="16" width="10.81640625" style="4"/>
+    <col min="1" max="1" width="10.85546875" style="2"/>
+    <col min="2" max="2" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.5703125" style="2" customWidth="1"/>
+    <col min="5" max="8" width="10.85546875" style="3"/>
+    <col min="9" max="9" width="11.42578125" style="3"/>
+    <col min="10" max="10" width="33.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="4" customWidth="1"/>
+    <col min="13" max="14" width="30.5703125" style="4" customWidth="1"/>
+    <col min="15" max="16" width="10.85546875" style="4"/>
     <col min="17" max="17" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" style="4" customWidth="1"/>
-    <col min="19" max="26" width="30.54296875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="76.81640625" style="4" customWidth="1"/>
+    <col min="19" max="26" width="30.5703125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="76.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
@@ -924,7 +924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
       <c r="B2" s="16"/>
       <c r="C2" s="1" t="s">
@@ -985,7 +985,7 @@
       </c>
       <c r="AA2" s="14"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1039,25 +1039,25 @@
         <v>666666666</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>17</v>
@@ -1066,7 +1066,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="9"/>
       <c r="C4" s="8"/>
@@ -1094,7 +1094,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="9"/>
       <c r="C5" s="8"/>
@@ -1122,7 +1122,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9"/>
       <c r="C6" s="8"/>
@@ -1150,7 +1150,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="9"/>
       <c r="C7" s="8"/>
@@ -1178,7 +1178,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="9"/>
       <c r="C8" s="8"/>
@@ -1206,7 +1206,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="9"/>
       <c r="C9" s="8"/>
@@ -1234,7 +1234,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="9"/>
       <c r="C10" s="8"/>
@@ -1262,7 +1262,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="9"/>
       <c r="C11" s="8"/>
@@ -1290,7 +1290,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9"/>
       <c r="C12" s="8"/>
@@ -1318,7 +1318,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="9"/>
       <c r="C13" s="8"/>
@@ -1346,7 +1346,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="9"/>
       <c r="C14" s="8"/>
@@ -1374,7 +1374,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
       <c r="C15" s="8"/>
@@ -1402,7 +1402,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="9"/>
       <c r="C16" s="8"/>
@@ -1430,7 +1430,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
@@ -1458,7 +1458,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9"/>
       <c r="C18" s="8"/>
@@ -1486,7 +1486,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="9"/>
       <c r="C19" s="8"/>
@@ -1514,7 +1514,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="9"/>
       <c r="C20" s="8"/>
@@ -1542,7 +1542,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="9"/>
       <c r="C21" s="8"/>
@@ -1570,7 +1570,7 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="9"/>
       <c r="C22" s="8"/>
@@ -1598,7 +1598,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="9"/>
       <c r="C23" s="8"/>
@@ -1626,7 +1626,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="9"/>
       <c r="C24" s="8"/>
@@ -1654,7 +1654,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="9"/>
       <c r="C25" s="8"/>
@@ -1682,7 +1682,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -1700,7 +1700,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -1718,7 +1718,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -1736,7 +1736,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -1754,7 +1754,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -1772,7 +1772,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1790,7 +1790,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1808,7 +1808,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1826,7 +1826,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -1844,7 +1844,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -1862,7 +1862,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -1880,7 +1880,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -1898,7 +1898,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -1916,7 +1916,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1934,7 +1934,7 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="11:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>

</xml_diff>

<commit_message>
fix (generador_pdf): markers relocated
</commit_message>
<xml_diff>
--- a/files/Data.xlsx
+++ b/files/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Molina\Documents\MEGA\+Generadores\PDF-Request-Generator-master\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abels\OneDrive\Desktop\PDF-Request-Generator\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EA588D-319B-4231-B01F-AAD2C20DE2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05962DAC-2CA8-4BCB-AE6C-325576435598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{7171335B-6EB2-4E13-BF21-E8880F3867D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7171335B-6EB2-4E13-BF21-E8880F3867D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -574,6 +574,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,21 +610,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,12 +617,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -639,7 +639,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -656,9 +656,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -696,7 +696,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -802,7 +802,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -944,7 +944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -954,96 +954,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F700F14-4C69-4246-A617-9B75CEA3E3EC}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.54296875" style="2" customWidth="1"/>
-    <col min="5" max="8" width="10.81640625" style="3"/>
-    <col min="9" max="9" width="11.453125" style="3"/>
-    <col min="10" max="10" width="33.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.453125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="32.7265625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="20.81640625" style="4" customWidth="1"/>
-    <col min="14" max="15" width="30.54296875" style="4" customWidth="1"/>
-    <col min="16" max="17" width="10.81640625" style="4"/>
+    <col min="1" max="1" width="10.85546875" style="2"/>
+    <col min="2" max="2" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.5703125" style="2" customWidth="1"/>
+    <col min="5" max="8" width="10.85546875" style="3"/>
+    <col min="9" max="9" width="11.42578125" style="3"/>
+    <col min="10" max="10" width="33.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="32.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="4" customWidth="1"/>
+    <col min="14" max="15" width="30.5703125" style="4" customWidth="1"/>
+    <col min="16" max="17" width="10.85546875" style="4"/>
     <col min="18" max="18" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" style="4" customWidth="1"/>
-    <col min="20" max="27" width="30.54296875" style="4" customWidth="1"/>
-    <col min="28" max="28" width="76.81640625" style="4" customWidth="1"/>
+    <col min="20" max="27" width="30.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="76.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="14" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="19"/>
-      <c r="B2" s="13"/>
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1068,15 +1068,15 @@
       <c r="J2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
       <c r="T2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1101,9 +1101,9 @@
       <c r="AA2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="15"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB2" s="22"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1166,37 +1166,29 @@
         <v>17</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:K2"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
@@ -1206,6 +1198,14 @@
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:AA1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N3" r:id="rId1" xr:uid="{E35BC787-B146-4C32-8CEC-1551AED2F649}"/>
@@ -1223,14 +1223,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="3"/>
-    <col min="2" max="2" width="29.1796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="3"/>
+    <col min="2" max="2" width="29.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>18</v>
       </c>
@@ -1241,12 +1241,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28"/>
       <c r="B2" s="30"/>
       <c r="C2" s="32"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <f>Hoja1!A3</f>
         <v>1</v>
@@ -1260,7 +1260,7 @@
         <v>XXXXXXXXE</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <f>Hoja1!A4</f>
         <v>0</v>
@@ -1274,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <f>Hoja1!A5</f>
         <v>0</v>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <f>Hoja1!A6</f>
         <v>0</v>
@@ -1302,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <f>Hoja1!A7</f>
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <f>Hoja1!A8</f>
         <v>0</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <f>Hoja1!A9</f>
         <v>0</v>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <f>Hoja1!A10</f>
         <v>0</v>
@@ -1358,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <f>Hoja1!A11</f>
         <v>0</v>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <f>Hoja1!A12</f>
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <f>Hoja1!A13</f>
         <v>0</v>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <f>Hoja1!A14</f>
         <v>0</v>
@@ -1414,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <f>Hoja1!A15</f>
         <v>0</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <f>Hoja1!A16</f>
         <v>0</v>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <f>Hoja1!A17</f>
         <v>0</v>
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <f>Hoja1!A18</f>
         <v>0</v>
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <f>Hoja1!A19</f>
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <f>Hoja1!A20</f>
         <v>0</v>
@@ -1498,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <f>Hoja1!A21</f>
         <v>0</v>
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <f>Hoja1!A22</f>
         <v>0</v>
@@ -1526,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <f>Hoja1!A23</f>
         <v>0</v>
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <f>Hoja1!A24</f>
         <v>0</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <f>Hoja1!A25</f>
         <v>0</v>
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <f>Hoja1!A26</f>
         <v>0</v>
@@ -1582,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <f>Hoja1!A27</f>
         <v>0</v>
@@ -1596,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <f>Hoja1!A28</f>
         <v>0</v>
@@ -1610,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <f>Hoja1!A29</f>
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <f>Hoja1!A30</f>
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <f>Hoja1!A31</f>
         <v>0</v>
@@ -1652,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <f>Hoja1!A32</f>
         <v>0</v>
@@ -1666,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <f>Hoja1!A33</f>
         <v>0</v>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <f>Hoja1!A34</f>
         <v>0</v>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <f>Hoja1!A35</f>
         <v>0</v>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <f>Hoja1!A36</f>
         <v>0</v>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <f>Hoja1!A37</f>
         <v>0</v>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <f>Hoja1!A38</f>
         <v>0</v>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <f>Hoja1!A39</f>
         <v>0</v>
@@ -1764,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <f>Hoja1!A40</f>
         <v>0</v>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <f>Hoja1!A41</f>
         <v>0</v>
@@ -1792,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <f>Hoja1!A42</f>
         <v>0</v>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <f>Hoja1!A43</f>
         <v>0</v>
@@ -1820,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <f>Hoja1!A44</f>
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <f>Hoja1!A45</f>
         <v>0</v>
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <f>Hoja1!A46</f>
         <v>0</v>
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <f>Hoja1!A47</f>
         <v>0</v>
@@ -1876,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <f>Hoja1!A48</f>
         <v>0</v>
@@ -1890,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <f>Hoja1!A49</f>
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <f>Hoja1!A50</f>
         <v>0</v>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <f>Hoja1!A51</f>
         <v>0</v>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <f>Hoja1!A52</f>
         <v>0</v>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <f>Hoja1!A53</f>
         <v>0</v>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <f>Hoja1!A54</f>
         <v>0</v>
@@ -1974,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <f>Hoja1!A55</f>
         <v>0</v>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <f>Hoja1!A56</f>
         <v>0</v>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <f>Hoja1!A57</f>
         <v>0</v>
@@ -2016,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <f>Hoja1!A58</f>
         <v>0</v>
@@ -2030,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <f>Hoja1!A59</f>
         <v>0</v>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <f>Hoja1!A60</f>
         <v>0</v>
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <f>Hoja1!A61</f>
         <v>0</v>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <f>Hoja1!A62</f>
         <v>0</v>
@@ -2086,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <f>Hoja1!A63</f>
         <v>0</v>
@@ -2100,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <f>Hoja1!A64</f>
         <v>0</v>
@@ -2114,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <f>Hoja1!A65</f>
         <v>0</v>
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <f>Hoja1!A66</f>
         <v>0</v>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <f>Hoja1!A67</f>
         <v>0</v>
@@ -2156,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <f>Hoja1!A68</f>
         <v>0</v>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <f>Hoja1!A69</f>
         <v>0</v>
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <f>Hoja1!A70</f>
         <v>0</v>
@@ -2198,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <f>Hoja1!A71</f>
         <v>0</v>
@@ -2212,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <f>Hoja1!A72</f>
         <v>0</v>
@@ -2226,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <f>Hoja1!A73</f>
         <v>0</v>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <f>Hoja1!A74</f>
         <v>0</v>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <f>Hoja1!A75</f>
         <v>0</v>
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <f>Hoja1!A76</f>
         <v>0</v>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <f>Hoja1!A77</f>
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="11">
         <f>Hoja1!A78</f>
         <v>0</v>
@@ -2310,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <f>Hoja1!A79</f>
         <v>0</v>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <f>Hoja1!A80</f>
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <f>Hoja1!A81</f>
         <v>0</v>
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <f>Hoja1!A82</f>
         <v>0</v>
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <f>Hoja1!A83</f>
         <v>0</v>
@@ -2380,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <f>Hoja1!A84</f>
         <v>0</v>
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <f>Hoja1!A85</f>
         <v>0</v>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <f>Hoja1!A86</f>
         <v>0</v>
@@ -2422,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <f>Hoja1!A87</f>
         <v>0</v>
@@ -2436,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <f>Hoja1!A88</f>
         <v>0</v>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <f>Hoja1!A89</f>
         <v>0</v>
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <f>Hoja1!A90</f>
         <v>0</v>
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <f>Hoja1!A91</f>
         <v>0</v>
@@ -2492,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <f>Hoja1!A92</f>
         <v>0</v>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <f>Hoja1!A93</f>
         <v>0</v>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <f>Hoja1!A94</f>
         <v>0</v>
@@ -2534,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <f>Hoja1!A95</f>
         <v>0</v>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <f>Hoja1!A96</f>
         <v>0</v>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <f>Hoja1!A97</f>
         <v>0</v>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
         <f>Hoja1!A98</f>
         <v>0</v>
@@ -2590,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <f>Hoja1!A99</f>
         <v>0</v>
@@ -2604,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <f>Hoja1!A100</f>
         <v>0</v>
@@ -2618,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <f>Hoja1!A101</f>
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <f>Hoja1!A102</f>
         <v>0</v>
@@ -2646,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="11">
         <f>Hoja1!A103</f>
         <v>0</v>
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="11">
         <f>Hoja1!A104</f>
         <v>0</v>
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="11">
         <f>Hoja1!A105</f>
         <v>0</v>
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="11">
         <f>Hoja1!A106</f>
         <v>0</v>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <f>Hoja1!A107</f>
         <v>0</v>
@@ -2716,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
         <f>Hoja1!A108</f>
         <v>0</v>
@@ -2730,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="11">
         <f>Hoja1!A109</f>
         <v>0</v>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <f>Hoja1!A110</f>
         <v>0</v>
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <f>Hoja1!A111</f>
         <v>0</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
         <f>Hoja1!A112</f>
         <v>0</v>
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
         <f>Hoja1!A113</f>
         <v>0</v>
@@ -2800,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="11">
         <f>Hoja1!A114</f>
         <v>0</v>
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <f>Hoja1!A115</f>
         <v>0</v>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="11">
         <f>Hoja1!A116</f>
         <v>0</v>
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <f>Hoja1!A117</f>
         <v>0</v>
@@ -2856,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="11">
         <f>Hoja1!A118</f>
         <v>0</v>
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="11">
         <f>Hoja1!A119</f>
         <v>0</v>
@@ -2884,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="11">
         <f>Hoja1!A120</f>
         <v>0</v>
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="11">
         <f>Hoja1!A121</f>
         <v>0</v>
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <f>Hoja1!A122</f>
         <v>0</v>
@@ -2926,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="11">
         <f>Hoja1!A123</f>
         <v>0</v>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="11">
         <f>Hoja1!A124</f>
         <v>0</v>
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="11">
         <f>Hoja1!A125</f>
         <v>0</v>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="11">
         <f>Hoja1!A126</f>
         <v>0</v>
@@ -2982,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="11">
         <f>Hoja1!A127</f>
         <v>0</v>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="11">
         <f>Hoja1!A128</f>
         <v>0</v>
@@ -3010,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="11">
         <f>Hoja1!A129</f>
         <v>0</v>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <f>Hoja1!A130</f>
         <v>0</v>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="11">
         <f>Hoja1!A131</f>
         <v>0</v>
@@ -3052,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="11">
         <f>Hoja1!A132</f>
         <v>0</v>
@@ -3066,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="11">
         <f>Hoja1!A133</f>
         <v>0</v>
@@ -3080,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="11">
         <f>Hoja1!A134</f>
         <v>0</v>
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="11">
         <f>Hoja1!A135</f>
         <v>0</v>
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="11">
         <f>Hoja1!A136</f>
         <v>0</v>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="11">
         <f>Hoja1!A137</f>
         <v>0</v>
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="11">
         <f>Hoja1!A138</f>
         <v>0</v>
@@ -3150,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="11">
         <f>Hoja1!A139</f>
         <v>0</v>
@@ -3164,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="11">
         <f>Hoja1!A140</f>
         <v>0</v>
@@ -3178,7 +3178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="11">
         <f>Hoja1!A141</f>
         <v>0</v>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="11">
         <f>Hoja1!A142</f>
         <v>0</v>
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="11">
         <f>Hoja1!A143</f>
         <v>0</v>
@@ -3220,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="11">
         <f>Hoja1!A144</f>
         <v>0</v>
@@ -3234,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="11">
         <f>Hoja1!A145</f>
         <v>0</v>
@@ -3248,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="11">
         <f>Hoja1!A146</f>
         <v>0</v>
@@ -3262,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="11">
         <f>Hoja1!A147</f>
         <v>0</v>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="11">
         <f>Hoja1!A148</f>
         <v>0</v>
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="11">
         <f>Hoja1!A149</f>
         <v>0</v>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="11">
         <f>Hoja1!A150</f>
         <v>0</v>
@@ -3318,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="11">
         <f>Hoja1!A151</f>
         <v>0</v>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="11">
         <f>Hoja1!A152</f>
         <v>0</v>
@@ -3346,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="11">
         <f>Hoja1!A153</f>
         <v>0</v>
@@ -3360,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="11">
         <f>Hoja1!A154</f>
         <v>0</v>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="11">
         <f>Hoja1!A155</f>
         <v>0</v>
@@ -3388,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="11">
         <f>Hoja1!A156</f>
         <v>0</v>
@@ -3402,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="11">
         <f>Hoja1!A157</f>
         <v>0</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="11">
         <f>Hoja1!A158</f>
         <v>0</v>
@@ -3430,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="11">
         <f>Hoja1!A159</f>
         <v>0</v>
@@ -3444,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="11">
         <f>Hoja1!A160</f>
         <v>0</v>
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="11">
         <f>Hoja1!A161</f>
         <v>0</v>
@@ -3472,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="11">
         <f>Hoja1!A162</f>
         <v>0</v>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="11">
         <f>Hoja1!A163</f>
         <v>0</v>
@@ -3500,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="11">
         <f>Hoja1!A164</f>
         <v>0</v>
@@ -3514,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="11">
         <f>Hoja1!A165</f>
         <v>0</v>
@@ -3528,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="11">
         <f>Hoja1!A166</f>
         <v>0</v>
@@ -3542,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="11">
         <f>Hoja1!A167</f>
         <v>0</v>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="11">
         <f>Hoja1!A168</f>
         <v>0</v>
@@ -3570,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="11">
         <f>Hoja1!A169</f>
         <v>0</v>
@@ -3584,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="11">
         <f>Hoja1!A170</f>
         <v>0</v>
@@ -3598,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="11">
         <f>Hoja1!A171</f>
         <v>0</v>
@@ -3612,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="11">
         <f>Hoja1!A172</f>
         <v>0</v>
@@ -3626,7 +3626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="11">
         <f>Hoja1!A173</f>
         <v>0</v>
@@ -3640,7 +3640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="11">
         <f>Hoja1!A174</f>
         <v>0</v>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="11">
         <f>Hoja1!A175</f>
         <v>0</v>
@@ -3668,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="11">
         <f>Hoja1!A176</f>
         <v>0</v>
@@ -3682,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="11">
         <f>Hoja1!A177</f>
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="11">
         <f>Hoja1!A178</f>
         <v>0</v>
@@ -3710,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="11">
         <f>Hoja1!A179</f>
         <v>0</v>
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="11">
         <f>Hoja1!A180</f>
         <v>0</v>
@@ -3738,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="11">
         <f>Hoja1!A181</f>
         <v>0</v>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="11">
         <f>Hoja1!A182</f>
         <v>0</v>
@@ -3766,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="11">
         <f>Hoja1!A183</f>
         <v>0</v>
@@ -3780,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="11">
         <f>Hoja1!A184</f>
         <v>0</v>
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="11">
         <f>Hoja1!A185</f>
         <v>0</v>
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="11">
         <f>Hoja1!A186</f>
         <v>0</v>
@@ -3822,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="11">
         <f>Hoja1!A187</f>
         <v>0</v>
@@ -3836,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="11">
         <f>Hoja1!A188</f>
         <v>0</v>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="11">
         <f>Hoja1!A189</f>
         <v>0</v>
@@ -3864,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="11">
         <f>Hoja1!A190</f>
         <v>0</v>
@@ -3878,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="11">
         <f>Hoja1!A191</f>
         <v>0</v>
@@ -3892,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="11">
         <f>Hoja1!A192</f>
         <v>0</v>
@@ -3906,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="11">
         <f>Hoja1!A193</f>
         <v>0</v>
@@ -3920,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="11">
         <f>Hoja1!A194</f>
         <v>0</v>
@@ -3934,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="11">
         <f>Hoja1!A195</f>
         <v>0</v>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="11">
         <f>Hoja1!A196</f>
         <v>0</v>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="11">
         <f>Hoja1!A197</f>
         <v>0</v>
@@ -3976,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="11">
         <f>Hoja1!A198</f>
         <v>0</v>
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="11">
         <f>Hoja1!A199</f>
         <v>0</v>
@@ -4004,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="11">
         <f>Hoja1!A200</f>
         <v>0</v>
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="11">
         <f>Hoja1!A201</f>
         <v>0</v>
@@ -4032,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="11">
         <f>Hoja1!A202</f>
         <v>0</v>
@@ -4046,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="11">
         <f>Hoja1!A203</f>
         <v>0</v>
@@ -4060,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="11">
         <f>Hoja1!A204</f>
         <v>0</v>
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="11">
         <f>Hoja1!A205</f>
         <v>0</v>
@@ -4088,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="11">
         <f>Hoja1!A206</f>
         <v>0</v>
@@ -4102,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="11">
         <f>Hoja1!A207</f>
         <v>0</v>
@@ -4116,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="11">
         <f>Hoja1!A208</f>
         <v>0</v>
@@ -4130,7 +4130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="11">
         <f>Hoja1!A209</f>
         <v>0</v>
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="11">
         <f>Hoja1!A210</f>
         <v>0</v>
@@ -4158,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="11">
         <f>Hoja1!A211</f>
         <v>0</v>
@@ -4172,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="11">
         <f>Hoja1!A212</f>
         <v>0</v>
@@ -4186,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="11">
         <f>Hoja1!A213</f>
         <v>0</v>
@@ -4200,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="11">
         <f>Hoja1!A214</f>
         <v>0</v>
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="11">
         <f>Hoja1!A215</f>
         <v>0</v>
@@ -4228,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="11">
         <f>Hoja1!A216</f>
         <v>0</v>
@@ -4242,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="11">
         <f>Hoja1!A217</f>
         <v>0</v>
@@ -4256,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="11">
         <f>Hoja1!A218</f>
         <v>0</v>
@@ -4270,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="11">
         <f>Hoja1!A219</f>
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="11">
         <f>Hoja1!A220</f>
         <v>0</v>
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="11">
         <f>Hoja1!A221</f>
         <v>0</v>
@@ -4312,7 +4312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="11">
         <f>Hoja1!A222</f>
         <v>0</v>
@@ -4326,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="11">
         <f>Hoja1!A223</f>
         <v>0</v>
@@ -4340,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="11">
         <f>Hoja1!A224</f>
         <v>0</v>
@@ -4354,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="11">
         <f>Hoja1!A225</f>
         <v>0</v>
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="11">
         <f>Hoja1!A226</f>
         <v>0</v>

</xml_diff>